<commit_message>
add vlaidaiton from Dom
</commit_message>
<xml_diff>
--- a/dat/validation/deps_to_validate.xlsx
+++ b/dat/validation/deps_to_validate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dglandorf/Documents/Studium/QDS/_ResearchProject/learning-dependencies/dat/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85B12B3-048C-EB4F-BACC-3CE890F9F75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9830738F-8AA0-B945-8FE0-127C4343EC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
     <t>Group (mathematics)</t>
   </si>
   <si>
-    <t>correct</t>
+    <t>correct (0/1)</t>
   </si>
 </sst>
 </file>
@@ -1117,14 +1117,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>